<commit_message>
added dueDate column to Project table
</commit_message>
<xml_diff>
--- a/design-requirements-text/database-sketch.xlsx
+++ b/design-requirements-text/database-sketch.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FCI\Level 3 - Sem1\IS\project-manager\design-requirements-text\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files (x86)\EasyPHP-Devserver-17\eds-www\project-manager\design-requirements-text\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F176B39-3041-4BD2-8479-7354A089F3E3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE75A1B3-E761-441E-BDF5-745FC32FA9A6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="18030" yWindow="3525" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="60">
   <si>
     <t>Project</t>
   </si>
@@ -202,6 +202,9 @@
   </si>
   <si>
     <t>This is only for Major Tasks. Need to check parenttask == null before inserting here</t>
+  </si>
+  <si>
+    <t>DueDate</t>
   </si>
 </sst>
 </file>
@@ -262,11 +265,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -547,10 +550,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q116"/>
+  <dimension ref="A1:O116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="E71" sqref="E71"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -567,10 +570,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="O1" s="4" t="s">
         <v>30</v>
       </c>
     </row>
@@ -594,6 +597,9 @@
         <v>5</v>
       </c>
       <c r="H2" t="s">
+        <v>59</v>
+      </c>
+      <c r="I2" t="s">
         <v>7</v>
       </c>
     </row>
@@ -620,6 +626,9 @@
         <v>14</v>
       </c>
       <c r="H3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3" t="s">
         <v>15</v>
       </c>
       <c r="O3" s="2" t="s">
@@ -650,7 +659,7 @@
       <c r="G5" t="s">
         <v>22</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>21</v>
       </c>
       <c r="O5" s="2" t="s">
@@ -679,7 +688,10 @@
       <c r="G6" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I6" t="s">
         <v>20</v>
       </c>
       <c r="O6" s="2" t="s">
@@ -723,31 +735,31 @@
       <c r="A12" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
       <c r="O12" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-    </row>
-    <row r="15" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+    </row>
+    <row r="15" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>25</v>
@@ -837,9 +849,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="30" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="5" t="s">
+      <c r="A31" s="4" t="s">
         <v>31</v>
       </c>
     </row>
@@ -977,9 +989,9 @@
         <v>36</v>
       </c>
     </row>
-    <row r="45" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="45" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A47" s="5" t="s">
+      <c r="A47" s="4" t="s">
         <v>37</v>
       </c>
     </row>
@@ -1061,9 +1073,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="60" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="60" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="5" t="s">
+      <c r="A61" s="4" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1142,15 +1154,15 @@
         <v>11</v>
       </c>
     </row>
-    <row r="74" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="74" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="76" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="76" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A77" s="5" t="s">
+      <c r="A77" s="4" t="s">
         <v>46</v>
       </c>
     </row>
@@ -1244,9 +1256,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="90" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="90" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A91" s="5" t="s">
+      <c r="A91" s="4" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1328,9 +1340,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="105" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="105" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="106" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A106" s="5"/>
+      <c r="A106" s="4"/>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109" s="3"/>

</xml_diff>

<commit_message>
added sql queries for creating tables, changes in database design
</commit_message>
<xml_diff>
--- a/design-requirements-text/database-sketch.xlsx
+++ b/design-requirements-text/database-sketch.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files (x86)\EasyPHP-Devserver-17\eds-www\project-manager\design-requirements-text\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE75A1B3-E761-441E-BDF5-745FC32FA9A6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50A3524F-AE74-4005-9A66-F42008ABF57E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18030" yWindow="3525" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7200" yWindow="3525" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="60">
   <si>
     <t>Project</t>
   </si>
@@ -93,9 +93,6 @@
     <t>Sunday</t>
   </si>
   <si>
-    <t>Today</t>
-  </si>
-  <si>
     <t>Total Days needed = summation of days needed of tasks</t>
   </si>
   <si>
@@ -156,9 +153,6 @@
     <t>TaskID</t>
   </si>
   <si>
-    <t>ActualDaysNeeded</t>
-  </si>
-  <si>
     <t>PlannedDays?</t>
   </si>
   <si>
@@ -205,6 +199,12 @@
   </si>
   <si>
     <t>DueDate</t>
+  </si>
+  <si>
+    <t>Today/couldn’t do it in mysql</t>
+  </si>
+  <si>
+    <t>DaysWorked</t>
   </si>
 </sst>
 </file>
@@ -228,7 +228,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -247,6 +247,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -262,7 +268,6 @@
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -270,6 +275,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -552,8 +558,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="A91" sqref="A91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -570,11 +576,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="O1" s="4" t="s">
-        <v>30</v>
+      <c r="O1" s="3" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
@@ -597,14 +603,14 @@
         <v>5</v>
       </c>
       <c r="H2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="I2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B3" t="s">
@@ -631,23 +637,23 @@
       <c r="I3" t="s">
         <v>15</v>
       </c>
-      <c r="O3" s="2" t="s">
+      <c r="O3" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="O4" s="2" t="s">
+      <c r="B4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="O4" s="1" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D5">
@@ -657,77 +663,77 @@
         <v>5</v>
       </c>
       <c r="G5" t="s">
-        <v>22</v>
+        <v>58</v>
       </c>
       <c r="I5" t="s">
         <v>21</v>
       </c>
-      <c r="O5" s="2" t="s">
+      <c r="O5" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H6" s="3" t="s">
+      <c r="B6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H6" s="2" t="s">
         <v>20</v>
       </c>
       <c r="I6" t="s">
         <v>20</v>
       </c>
-      <c r="O6" s="2" t="s">
+      <c r="O6" s="1" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="O7" s="2" t="s">
+      <c r="B7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="O7" s="1" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="O8" s="2" t="s">
+      <c r="O8" s="1" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>38</v>
-      </c>
-      <c r="O10" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="O10" s="1" t="s">
         <v>10</v>
       </c>
     </row>
@@ -735,37 +741,37 @@
       <c r="A12" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
+      <c r="B12" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
       <c r="O12" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+    </row>
+    <row r="15" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
-    </row>
-    <row r="15" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>1</v>
       </c>
@@ -773,41 +779,41 @@
         <v>2</v>
       </c>
       <c r="D18" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19" t="s">
+        <v>12</v>
+      </c>
+      <c r="C19" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B19" t="s">
-        <v>12</v>
-      </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
         <v>27</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E19" t="s">
         <v>28</v>
       </c>
-      <c r="E19" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B20" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B22" t="s">
@@ -816,9 +822,12 @@
       <c r="C22" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
+      <c r="E22" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B23" t="s">
@@ -828,34 +837,34 @@
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
         <v>19</v>
       </c>
       <c r="E24" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B26" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="30" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>1</v>
       </c>
@@ -863,139 +872,133 @@
         <v>2</v>
       </c>
       <c r="D32" t="s">
+        <v>31</v>
+      </c>
+      <c r="E32" t="s">
+        <v>5</v>
+      </c>
+      <c r="F32" t="s">
+        <v>28</v>
+      </c>
+      <c r="G32" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B34" t="s">
+        <v>12</v>
+      </c>
+      <c r="C34" t="s">
         <v>26</v>
       </c>
-      <c r="E32" t="s">
+      <c r="D34" t="s">
+        <v>12</v>
+      </c>
+      <c r="E34" t="s">
         <v>32</v>
       </c>
-      <c r="F32" t="s">
-        <v>5</v>
-      </c>
-      <c r="G32" t="s">
-        <v>29</v>
-      </c>
-      <c r="H32" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B34" t="s">
-        <v>12</v>
-      </c>
-      <c r="C34" t="s">
-        <v>27</v>
-      </c>
-      <c r="D34" t="s">
-        <v>28</v>
-      </c>
-      <c r="E34" t="s">
-        <v>12</v>
-      </c>
       <c r="F34" t="s">
+        <v>12</v>
+      </c>
+      <c r="G34" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B35" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E36" t="s">
         <v>33</v>
       </c>
-      <c r="G34" t="s">
-        <v>12</v>
-      </c>
-      <c r="H34" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B35" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F36" t="s">
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B37" t="s">
+        <v>20</v>
+      </c>
+      <c r="C37" t="s">
+        <v>20</v>
+      </c>
+      <c r="D37" t="s">
+        <v>20</v>
+      </c>
+      <c r="E37" t="s">
+        <v>20</v>
+      </c>
+      <c r="F37" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B38" t="s">
+        <v>20</v>
+      </c>
+      <c r="C38" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F39" t="s">
+        <v>0</v>
+      </c>
+      <c r="G39" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B41" t="s">
+        <v>37</v>
+      </c>
+      <c r="E41" t="s">
+        <v>40</v>
+      </c>
+      <c r="F41" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B37" t="s">
-        <v>20</v>
-      </c>
-      <c r="C37" t="s">
-        <v>20</v>
-      </c>
-      <c r="E37" t="s">
-        <v>20</v>
-      </c>
-      <c r="F37" t="s">
-        <v>20</v>
-      </c>
-      <c r="G37" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B38" t="s">
-        <v>20</v>
-      </c>
-      <c r="C38" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G39" t="s">
-        <v>0</v>
-      </c>
-      <c r="H39" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B41" t="s">
-        <v>38</v>
-      </c>
-      <c r="F41" t="s">
-        <v>41</v>
-      </c>
-      <c r="G41" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F42" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E42" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>11</v>
       </c>
       <c r="B43" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" s="6" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="45" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A47" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
         <v>1</v>
       </c>
@@ -1003,25 +1006,25 @@
         <v>2</v>
       </c>
       <c r="D48" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="2" t="s">
+      <c r="A49" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B49" t="s">
         <v>12</v>
       </c>
       <c r="C49" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D49" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="2" t="s">
+      <c r="A50" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B50" t="s">
@@ -1029,12 +1032,12 @@
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="2" t="s">
+      <c r="A51" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="2" t="s">
+      <c r="A52" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B52" t="s">
@@ -1048,7 +1051,7 @@
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="2" t="s">
+      <c r="A53" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B53" t="s">
@@ -1056,16 +1059,16 @@
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="2" t="s">
+      <c r="A54" s="1" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="2" t="s">
+      <c r="A56" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B56" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
@@ -1073,49 +1076,49 @@
         <v>11</v>
       </c>
     </row>
-    <row r="60" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="60" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="4" t="s">
-        <v>40</v>
+      <c r="A61" s="6" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
+        <v>41</v>
+      </c>
+      <c r="C62" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B63" t="s">
+        <v>12</v>
+      </c>
+      <c r="C63" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B64" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C65" t="s">
         <v>42</v>
       </c>
-      <c r="C62" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B63" t="s">
-        <v>12</v>
-      </c>
-      <c r="C63" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B64" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A65" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C65" t="s">
-        <v>44</v>
-      </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A66" s="2" t="s">
+      <c r="A66" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B66" t="s">
@@ -1126,7 +1129,7 @@
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A67" s="2" t="s">
+      <c r="A67" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B67" t="s">
@@ -1134,19 +1137,19 @@
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A68" s="2" t="s">
+      <c r="A68" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B68" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A70" s="2" t="s">
+      <c r="A70" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E70" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
@@ -1154,101 +1157,101 @@
         <v>11</v>
       </c>
     </row>
-    <row r="74" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="74" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A77" s="4" t="s">
-        <v>46</v>
+      <c r="A77" s="6" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B78" t="s">
+        <v>45</v>
+      </c>
+      <c r="C78" t="s">
+        <v>41</v>
+      </c>
+      <c r="D78" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A79" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B79" t="s">
+        <v>12</v>
+      </c>
+      <c r="C79" t="s">
+        <v>12</v>
+      </c>
+      <c r="D79" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A80" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B80" t="s">
+        <v>20</v>
+      </c>
+      <c r="C80" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B82" t="s">
+        <v>20</v>
+      </c>
+      <c r="C82" t="s">
+        <v>20</v>
+      </c>
+      <c r="D82" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B83" t="s">
+        <v>20</v>
+      </c>
+      <c r="C83" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B84" t="s">
         <v>47</v>
       </c>
-      <c r="C78" t="s">
-        <v>42</v>
-      </c>
-      <c r="D78" t="s">
+      <c r="C84" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A86" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D86" t="s">
         <v>48</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A79" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B79" t="s">
-        <v>12</v>
-      </c>
-      <c r="C79" t="s">
-        <v>12</v>
-      </c>
-      <c r="D79" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A80" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B80" t="s">
-        <v>20</v>
-      </c>
-      <c r="C80" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B82" t="s">
-        <v>20</v>
-      </c>
-      <c r="C82" t="s">
-        <v>20</v>
-      </c>
-      <c r="D82" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A83" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B83" t="s">
-        <v>20</v>
-      </c>
-      <c r="C83" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A84" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B84" t="s">
-        <v>49</v>
-      </c>
-      <c r="C84" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A86" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D86" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
@@ -1256,83 +1259,83 @@
         <v>11</v>
       </c>
     </row>
-    <row r="90" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="90" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A91" s="4" t="s">
-        <v>51</v>
+      <c r="A91" s="6" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B93" t="s">
+        <v>50</v>
+      </c>
+      <c r="C93" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A94" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B94" t="s">
+        <v>12</v>
+      </c>
+      <c r="C94" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A95" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B95" t="s">
+        <v>20</v>
+      </c>
+      <c r="C95" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A97" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B97" t="s">
+        <v>20</v>
+      </c>
+      <c r="C97" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A98" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A99" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B99" t="s">
+        <v>30</v>
+      </c>
+      <c r="C99" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A101" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D101" t="s">
         <v>52</v>
       </c>
-      <c r="C93" t="s">
+      <c r="F101" t="s">
         <v>53</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A94" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B94" t="s">
-        <v>12</v>
-      </c>
-      <c r="C94" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A95" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B95" t="s">
-        <v>20</v>
-      </c>
-      <c r="C95" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A96" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A97" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B97" t="s">
-        <v>20</v>
-      </c>
-      <c r="C97" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A98" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A99" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B99" t="s">
-        <v>31</v>
-      </c>
-      <c r="C99" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A101" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D101" t="s">
-        <v>54</v>
-      </c>
-      <c r="F101" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
@@ -1340,33 +1343,33 @@
         <v>11</v>
       </c>
     </row>
-    <row r="105" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="105" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="106" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A106" s="4"/>
+      <c r="A106" s="3"/>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A109" s="3"/>
+      <c r="A109" s="2"/>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A110" s="3"/>
+      <c r="A110" s="2"/>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A111" s="3"/>
+      <c r="A111" s="2"/>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A112" s="3"/>
+      <c r="A112" s="2"/>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A113" s="3"/>
+      <c r="A113" s="2"/>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A114" s="3"/>
+      <c r="A114" s="2"/>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A115" s="3"/>
+      <c r="A115" s="2"/>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A116" s="3"/>
+      <c r="A116" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>